<commit_message>
Made changes in Config.py
</commit_message>
<xml_diff>
--- a/test_data/test_data.xlsx
+++ b/test_data/test_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\OrangeHRM\Test_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\OrangeHRM\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71BED1AC-1F0B-4F1A-93D2-DB3506B858BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C99F37-18E9-4BEF-ADE2-A8F957B675BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -51,30 +51,12 @@
     <t>https://opensource-demo.orangehrmlive.com/</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>txtUsername</t>
-  </si>
-  <si>
     <t>Admin</t>
   </si>
   <si>
-    <t>txtPassword</t>
-  </si>
-  <si>
     <t>admin123</t>
   </si>
   <si>
-    <t>btnLogin</t>
-  </si>
-  <si>
-    <t>welcome</t>
-  </si>
-  <si>
-    <t>Welcome Admin</t>
-  </si>
-  <si>
     <t>enter_username</t>
   </si>
   <si>
@@ -88,6 +70,27 @@
   </si>
   <si>
     <t>verify_login</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>xpath</t>
+  </si>
+  <si>
+    <t>//button[@type='submit' and contains(@class, 'orangehrm-login-button')]</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>//h6[contains(@class, 'oxd-topbar-header-breadcrumb-module') and text()='Dashboard']</t>
   </si>
 </sst>
 </file>
@@ -132,13 +135,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -424,7 +436,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,8 +444,8 @@
     <col min="1" max="1" width="11.28515625" customWidth="1"/>
     <col min="2" max="2" width="16.140625" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="4" max="4" width="38.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -453,36 +465,36 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -490,53 +502,53 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
         <v>20</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{C2EE5156-C14E-46DC-9644-26F0297B0C05}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{A0AD3F29-651A-43A3-8329-45BB62E66113}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>